<commit_message>
MySql Database and Tables Created
</commit_message>
<xml_diff>
--- a/PlanningDataModels.xlsx
+++ b/PlanningDataModels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming\c#\my-projects\e-commerce-api\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143EC87D-3EE2-4AD1-B501-9F31D674A31C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750FC1F1-630E-4960-9703-D4DE2411D490}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{098B2945-9F56-457B-9815-D82E75202EBD}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="32">
   <si>
     <t>Product</t>
   </si>
@@ -118,6 +118,9 @@
   </si>
   <si>
     <t>C# Models API: EcommerceApi</t>
+  </si>
+  <si>
+    <t>nvarchar(120)</t>
   </si>
 </sst>
 </file>
@@ -181,14 +184,14 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -512,7 +515,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,65 +531,65 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="D3" s="2" t="s">
+      <c r="B3" s="3"/>
+      <c r="D3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="G3" s="2" t="s">
+      <c r="E3" s="3"/>
+      <c r="G3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="2"/>
-      <c r="J3" s="2" t="s">
+      <c r="H3" s="3"/>
+      <c r="J3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="2"/>
+      <c r="K3" s="3"/>
       <c r="M3" s="6" t="s">
         <v>28</v>
       </c>
       <c r="N3" s="6"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="s">
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" s="3" t="s">
+      <c r="H4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -597,22 +600,22 @@
       <c r="B5" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="H5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="K5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="M5" s="5" t="s">
@@ -683,61 +686,61 @@
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="D15" s="2" t="s">
+      <c r="B15" s="3"/>
+      <c r="D15" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="G15" s="2" t="s">
+      <c r="E15" s="3"/>
+      <c r="G15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H15" s="2"/>
-      <c r="J15" s="2" t="s">
+      <c r="H15" s="3"/>
+      <c r="J15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K15" s="2"/>
+      <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="B16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16" s="3" t="s">
+      <c r="E16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H16" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J16" s="3" t="s">
+      <c r="H16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K16" s="3" t="s">
+      <c r="K16" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -748,16 +751,16 @@
       <c r="B17" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J17" s="4" t="s">
+      <c r="E17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="K17" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -766,12 +769,12 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="E18" s="2" t="s">
         <v>3</v>
       </c>
       <c r="J18" t="s">

</xml_diff>